<commit_message>
during meeting with Rohit
</commit_message>
<xml_diff>
--- a/test data/tests solved manually.xlsx
+++ b/test data/tests solved manually.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\research\Covid19 POM Special\IJoC\writing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\VSCode\MatchingPPE\test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D6361C-B8BC-4D62-BA28-5EBD0C59EC39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F05B423-50CB-47CE-ADA6-96C0D7C77A56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15460" xr2:uid="{70FEA858-70CA-47A0-9FC4-770E64961922}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{70FEA858-70CA-47A0-9FC4-770E64961922}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="2" r:id="rId1"/>
@@ -530,9 +530,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,7 +570,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,39 +887,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B812AE96-95A2-4E8C-A470-D3A314DC5A9D}">
   <dimension ref="A2:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T49" sqref="T49"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
-    <col min="3" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.734375" customWidth="1"/>
+    <col min="3" max="6" width="11.15625" customWidth="1"/>
+    <col min="7" max="7" width="18.5234375" customWidth="1"/>
+    <col min="11" max="11" width="21.734375" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+    </row>
+    <row r="3" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="D4" s="43" t="s">
         <v>19</v>
       </c>
@@ -940,7 +938,7 @@
       </c>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="D5" s="10" t="s">
         <v>43</v>
       </c>
@@ -973,7 +971,7 @@
       </c>
       <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C6">
         <v>0</v>
       </c>
@@ -1005,7 +1003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C7">
         <v>1</v>
       </c>
@@ -1037,7 +1035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C8">
         <v>2</v>
       </c>
@@ -1069,8 +1067,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="12" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C12" s="43" t="s">
         <v>17</v>
       </c>
@@ -1078,7 +1076,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
         <v>0</v>
@@ -1090,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C15" s="14" t="s">
         <v>4</v>
       </c>
@@ -1118,15 +1116,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="46" t="s">
+    <row r="16" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="17" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C17" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="49"/>
       <c r="H17" t="s">
         <v>54</v>
       </c>
@@ -1134,7 +1132,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="10" t="s">
         <v>52</v>
       </c>
@@ -1169,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="4">
         <v>0</v>
       </c>
@@ -1218,7 +1216,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="4">
         <v>0</v>
       </c>
@@ -1266,7 +1264,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="4">
         <v>1</v>
       </c>
@@ -1314,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="4">
         <v>1</v>
       </c>
@@ -1362,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C23" s="7">
         <v>2</v>
       </c>
@@ -1410,12 +1408,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="21" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="C28" s="41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1429,7 +1427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" t="s">
         <v>4</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" t="s">
         <v>4</v>
       </c>
@@ -1456,23 +1454,23 @@
       <c r="R32" t="s">
         <v>0</v>
       </c>
-      <c r="S32" s="55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S32" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="J33" t="s">
         <v>63</v>
       </c>
       <c r="R33" t="s">
         <v>1</v>
       </c>
-      <c r="S33" s="55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S33" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="35" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
         <v>58</v>
       </c>
@@ -1491,12 +1489,12 @@
       <c r="R35" t="s">
         <v>67</v>
       </c>
-      <c r="S35" s="55">
+      <c r="S35" s="42">
         <f>SUMPRODUCT(F19:F23,J19:J23)/SUM(F19:F23)</f>
         <v>68.75</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="D36" s="10" t="s">
         <v>43</v>
       </c>
@@ -1524,12 +1522,12 @@
       <c r="R36" t="s">
         <v>68</v>
       </c>
-      <c r="S36" s="55">
+      <c r="S36" s="42">
         <f>SUMPRODUCT(L19:L23,F19:F23)/SUM(F19:F23)</f>
         <v>2.125</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C37">
         <v>0</v>
       </c>
@@ -1566,12 +1564,12 @@
       <c r="R37" t="s">
         <v>69</v>
       </c>
-      <c r="S37" s="55">
+      <c r="S37" s="42">
         <f>5/2</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="34">
         <v>1</v>
       </c>
@@ -1606,7 +1604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C39">
         <v>2</v>
       </c>
@@ -1638,17 +1636,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="R41" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="21" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="C42" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="R43">
         <v>11</v>
       </c>
@@ -1659,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="D45" t="s">
         <v>4</v>
       </c>
@@ -1705,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="R46">
         <v>11</v>
       </c>
@@ -1716,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B47" t="s">
         <v>62</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="D48" s="10" t="s">
         <v>43</v>
       </c>
@@ -1768,7 +1766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" s="34">
         <v>0</v>
       </c>
@@ -1808,11 +1806,11 @@
       <c r="R49" t="s">
         <v>71</v>
       </c>
-      <c r="T49" s="55">
+      <c r="T49" s="42">
         <v>2.5</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" s="34">
         <v>1</v>
       </c>
@@ -1850,7 +1848,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C51" s="34">
         <v>2</v>
       </c>
@@ -1909,39 +1907,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15C1A8-99E9-4808-B30E-7A7FB56C0447}">
   <dimension ref="A2:X71"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="3" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" customWidth="1"/>
+    <col min="3" max="6" width="11.15625" customWidth="1"/>
+    <col min="7" max="7" width="18.5234375" customWidth="1"/>
+    <col min="11" max="11" width="21.734375" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+    </row>
+    <row r="3" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C4" s="43" t="s">
         <v>18</v>
       </c>
@@ -1962,7 +1960,7 @@
       </c>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C5" s="10" t="s">
         <v>47</v>
       </c>
@@ -1995,7 +1993,7 @@
       </c>
       <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2032,7 +2030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
@@ -2151,8 +2149,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="12" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C12" s="43" t="s">
         <v>17</v>
       </c>
@@ -2160,7 +2158,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
         <v>0</v>
@@ -2172,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
@@ -2186,7 +2184,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C15" s="14" t="s">
         <v>4</v>
       </c>
@@ -2200,17 +2198,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="46" t="s">
+    <row r="16" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="17" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C17" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="49"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="10" t="s">
         <v>43</v>
       </c>
@@ -2245,7 +2243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="str">
         <f>_xlfn.CONCAT(C19,E19)</f>
         <v>D1gloves</v>
@@ -2290,7 +2288,7 @@
         <v>D1R1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="str">
         <f t="shared" ref="B20:B23" si="2">_xlfn.CONCAT(C20,E20)</f>
         <v>D1gloves</v>
@@ -2334,7 +2332,7 @@
         <v>D1R2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="str">
         <f t="shared" si="2"/>
         <v>D1gowns</v>
@@ -2378,7 +2376,7 @@
         <v>D2R1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="str">
         <f t="shared" si="2"/>
         <v>D2masks</v>
@@ -2422,7 +2420,7 @@
         <v>D2R2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B23" t="str">
         <f t="shared" si="2"/>
         <v>D2gowns</v>
@@ -2463,14 +2461,14 @@
         <v>D2R2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A38" s="52" t="s">
+    <row r="37" spans="1:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="53" t="s">
         <v>10</v>
       </c>
       <c r="B38" s="2"/>
@@ -2498,8 +2496,8 @@
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A39" s="53"/>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="54"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
         <v>0</v>
@@ -2532,8 +2530,8 @@
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="54"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>0</v>
@@ -2564,8 +2562,8 @@
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A41" s="53"/>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="54"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2591,8 +2589,8 @@
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="54"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
         <v>1</v>
@@ -2623,8 +2621,8 @@
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A43" s="53"/>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="54"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
         <v>1</v>
@@ -2655,8 +2653,8 @@
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="54"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2680,8 +2678,8 @@
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A45" s="53"/>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="54"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
         <v>2</v>
@@ -2712,8 +2710,8 @@
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
     </row>
-    <row r="46" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="54"/>
+    <row r="46" spans="1:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A46" s="55"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -2737,9 +2735,9 @@
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
     </row>
-    <row r="49" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="49" t="s">
+    <row r="49" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="50" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="2"/>
@@ -2761,8 +2759,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="50"/>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="51"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
@@ -2790,8 +2788,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" s="50"/>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="51"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5" t="s">
@@ -2817,8 +2815,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="50"/>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="51"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5" t="s">
@@ -2841,8 +2839,8 @@
       <c r="K53" s="6"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="50"/>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="51"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2855,8 +2853,8 @@
       <c r="K54" s="6"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="50"/>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="51"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2871,8 +2869,8 @@
       <c r="K55" s="6"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" s="50"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="51"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="15" t="s">
@@ -2892,8 +2890,8 @@
       <c r="K56" s="6"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" s="50"/>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="51"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5" t="s">
@@ -2918,8 +2916,8 @@
       <c r="K57" s="6"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" s="50"/>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="51"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5" t="s">
@@ -2942,8 +2940,8 @@
       <c r="K58" s="6"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="51"/>
+    <row r="59" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A59" s="52"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8" t="s">
@@ -2961,7 +2959,7 @@
       <c r="K59" s="9"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -2974,7 +2972,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -2987,9 +2985,9 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" s="49" t="s">
+    <row r="62" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="50" t="s">
         <v>26</v>
       </c>
       <c r="B63" s="2"/>
@@ -3007,8 +3005,8 @@
       <c r="J63" s="2"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="50"/>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="51"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
@@ -3030,8 +3028,8 @@
       <c r="J64" s="5"/>
       <c r="K64" s="6"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="50"/>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="51"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -3043,8 +3041,8 @@
       <c r="J65" s="5"/>
       <c r="K65" s="6"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="50"/>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="51"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -3056,8 +3054,8 @@
       <c r="J66" s="5"/>
       <c r="K66" s="6"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="50"/>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="51"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="15" t="s">
@@ -3073,8 +3071,8 @@
       <c r="J67" s="5"/>
       <c r="K67" s="6"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="50"/>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="51"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5" t="s">
@@ -3094,8 +3092,8 @@
       <c r="J68" s="5"/>
       <c r="K68" s="6"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="50"/>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="51"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -3107,8 +3105,8 @@
       <c r="J69" s="5"/>
       <c r="K69" s="6"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="50"/>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="51"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -3122,8 +3120,8 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="51"/>
+    <row r="71" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A71" s="52"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>

</xml_diff>

<commit_message>
need to fix dependencies
The scripts under scripts won't find the package ppematch
</commit_message>
<xml_diff>
--- a/test data/tests solved manually.xlsx
+++ b/test data/tests solved manually.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\VSCode\MatchingPPE\test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F05B423-50CB-47CE-ADA6-96C0D7C77A56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B312FFCE-9341-4E03-90F2-10A22AD16A18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{70FEA858-70CA-47A0-9FC4-770E64961922}"/>
+    <workbookView xWindow="4170" yWindow="4170" windowWidth="28800" windowHeight="15160" activeTab="1" xr2:uid="{70FEA858-70CA-47A0-9FC4-770E64961922}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="2" r:id="rId1"/>
-    <sheet name="test 2" sheetId="1" r:id="rId2"/>
+    <sheet name="Section 3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -206,9 +206,6 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>Shipping decisions</t>
-  </si>
-  <si>
     <t>Make matching decisions here ---&gt;</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>so, avg shipments</t>
+  </si>
+  <si>
+    <t>Matching decisions</t>
   </si>
 </sst>
 </file>
@@ -889,16 +889,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.734375" customWidth="1"/>
-    <col min="3" max="6" width="11.15625" customWidth="1"/>
-    <col min="7" max="7" width="18.5234375" customWidth="1"/>
-    <col min="11" max="11" width="21.734375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="3" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>32</v>
       </c>
@@ -910,14 +910,14 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D4" s="43" t="s">
         <v>19</v>
       </c>
@@ -938,7 +938,7 @@
       </c>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D5" s="10" t="s">
         <v>43</v>
       </c>
@@ -971,7 +971,7 @@
       </c>
       <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>0</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8">
         <v>2</v>
       </c>
@@ -1067,8 +1067,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="12" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="43" t="s">
         <v>17</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="14" t="s">
         <v>4</v>
       </c>
@@ -1116,28 +1116,28 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="17" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
       <c r="G17" s="49"/>
       <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
         <v>54</v>
       </c>
-      <c r="I17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>45</v>
@@ -1167,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C19" s="4">
         <v>0</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C20" s="4">
         <v>0</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C21" s="4">
         <v>1</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C22" s="4">
         <v>1</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="7">
         <v>2</v>
       </c>
@@ -1408,14 +1408,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:19" ht="21" x14ac:dyDescent="0.5">
       <c r="C28" s="41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
@@ -1427,7 +1427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>4</v>
       </c>
@@ -1438,10 +1438,10 @@
         <v>50</v>
       </c>
       <c r="R31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>4</v>
       </c>
@@ -1458,9 +1458,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R33" t="s">
         <v>1</v>
@@ -1469,10 +1469,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="35" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" s="43" t="s">
         <v>19</v>
@@ -1487,14 +1487,14 @@
       <c r="L35" s="44"/>
       <c r="M35" s="45"/>
       <c r="R35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S35" s="42">
         <f>SUMPRODUCT(F19:F23,J19:J23)/SUM(F19:F23)</f>
         <v>68.75</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D36" s="10" t="s">
         <v>43</v>
       </c>
@@ -1520,14 +1520,14 @@
         <v>46</v>
       </c>
       <c r="R36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S36" s="42">
         <f>SUMPRODUCT(L19:L23,F19:F23)/SUM(F19:F23)</f>
         <v>2.125</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C37">
         <v>0</v>
       </c>
@@ -1559,17 +1559,17 @@
         <v>0</v>
       </c>
       <c r="N37" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S37" s="42">
         <f>5/2</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C38" s="34">
         <v>1</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -1604,7 +1604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39">
         <v>2</v>
       </c>
@@ -1636,17 +1636,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="21" x14ac:dyDescent="0.5">
       <c r="C42" s="41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R43">
         <v>11</v>
       </c>
@@ -1657,9 +1657,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" t="s">
         <v>3</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>100</v>
       </c>
       <c r="J45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R45">
         <v>11</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="R46">
         <v>11</v>
       </c>
@@ -1714,9 +1714,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="43" t="s">
         <v>19</v>
@@ -1740,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D48" s="10" t="s">
         <v>43</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C49" s="34">
         <v>0</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -1801,16 +1801,16 @@
         <v>0</v>
       </c>
       <c r="N49" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T49" s="42">
         <v>2.5</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C50" s="34">
         <v>1</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -1845,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="N50" s="34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="3:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="34">
         <v>2</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I51">
         <v>2</v>
@@ -1883,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="N51" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1904,23 +1904,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15C1A8-99E9-4808-B30E-7A7FB56C0447}">
-  <dimension ref="A2:X71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36D9AB9-52BE-408F-931F-13381C764FB3}">
+  <dimension ref="A2:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="3" max="6" width="11.15625" customWidth="1"/>
-    <col min="7" max="7" width="18.5234375" customWidth="1"/>
-    <col min="11" max="11" width="21.734375" customWidth="1"/>
+    <col min="3" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:22" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>32</v>
       </c>
@@ -1932,14 +1932,14 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="43" t="s">
         <v>18</v>
       </c>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="10" t="s">
         <v>47</v>
       </c>
@@ -1993,9 +1993,9 @@
       </c>
       <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
@@ -2030,7 +2030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>300</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>3</v>
@@ -2067,7 +2067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
@@ -2149,8 +2149,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="12" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="43" t="s">
         <v>17</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
         <v>0</v>
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="14" t="s">
         <v>4</v>
       </c>
@@ -2198,17 +2198,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="17" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
       <c r="C17" s="47" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
       <c r="G17" s="49"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C18" s="10" t="s">
         <v>43</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f>_xlfn.CONCAT(C19,E19)</f>
         <v>D1gloves</v>
@@ -2288,7 +2291,7 @@
         <v>D1R1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f t="shared" ref="B20:B23" si="2">_xlfn.CONCAT(C20,E20)</f>
         <v>D1gloves</v>
@@ -2332,7 +2335,7 @@
         <v>D1R2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f t="shared" si="2"/>
         <v>D1gowns</v>
@@ -2376,7 +2379,7 @@
         <v>D2R1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B22" t="str">
         <f t="shared" si="2"/>
         <v>D2masks</v>
@@ -2420,7 +2423,7 @@
         <v>D2R2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" t="str">
         <f t="shared" si="2"/>
         <v>D2gowns</v>
@@ -2461,385 +2464,569 @@
         <v>D2R2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="53" t="s">
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A27" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="11" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="54"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A28" s="54"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="20">
-        <f>IF(D39="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D39,$D$19:$D$23,C39)/SUMIFS($F$6:$F$10,$E$6:$E$10,D39,$C$6:$C$10,C39)))</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="5" t="s">
+      <c r="E28" s="20">
+        <f>IF(D28="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D28,$D$19:$D$23,C28)/SUMIFS($F$6:$F$10,$E$6:$E$10,D28,$C$6:$C$10,C28)))</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A29" s="54"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="20">
+        <f>IF(D29="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D29,$D$19:$D$23,C29)/SUMIFS($F$6:$F$10,$E$6:$E$10,D29,$C$6:$C$10,C29)))</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A30" s="54"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A31" s="54"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="20">
+        <f>IF(D31="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D31,$D$19:$D$23,C31)/SUMIFS($F$6:$F$10,$E$6:$E$10,D31,$C$6:$C$10,C31)))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A32" s="54"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="20">
+        <f>IF(D32="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D32,$D$19:$D$23,C32)/SUMIFS($F$6:$F$10,$E$6:$E$10,D32,$C$6:$C$10,C32)))</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="54"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" s="54"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="20">
+        <f>IF(D34="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D34,$D$19:$D$23,C34)/SUMIFS($F$6:$F$10,$E$6:$E$10,D34,$C$6:$C$10,C34)))</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+    </row>
+    <row r="35" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="55"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+    </row>
+    <row r="38" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A39" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="2"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="54"/>
+      <c r="N39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A40" s="51"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="20">
-        <f>IF(D40="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D40,$D$19:$D$23,C40)/SUMIFS($F$6:$F$10,$E$6:$E$10,D40,$C$6:$C$10,C40)))</f>
-        <v>1</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E40" s="21">
+        <f>AVERAGEIF($D$28:$D$35,D40,$E$28:$E$35)</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
+      <c r="I40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="23">
+        <f>SUMIF($E$19:$E$23,I40,$I$19:$I$23)/SUMIF($E$19:$E$23,I40,$F$19:$F$23)</f>
+        <v>50</v>
+      </c>
+      <c r="K40" s="6"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="54"/>
+      <c r="N40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A41" s="51"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="D41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="21">
+        <f>AVERAGEIF($D$28:$D$35,D41,$E$28:$E$35)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
+      <c r="I41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="23">
+        <f>SUMIF($E$19:$E$23,I41,$I$19:$I$23)/SUMIF($E$19:$E$23,I41,$F$19:$F$23)</f>
+        <v>100</v>
+      </c>
+      <c r="K41" s="6"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="54"/>
+      <c r="N41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A42" s="51"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="20">
-        <f>IF(D42="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D42,$D$19:$D$23,C42)/SUMIFS($F$6:$F$10,$E$6:$E$10,D42,$C$6:$C$10,C42)))</f>
+        <v>7</v>
+      </c>
+      <c r="E42" s="21">
+        <f>AVERAGEIF($D$28:$D$35,D42,$E$28:$E$35)</f>
         <v>0.5</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="I42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="23">
+        <f>SUMIF($E$19:$E$23,I42,$I$19:$I$23)/SUMIF($E$19:$E$23,I42,$F$19:$F$23)</f>
+        <v>70</v>
+      </c>
+      <c r="K42" s="6"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="54"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A43" s="51"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="20">
-        <f>IF(D43="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D43,$D$19:$D$23,C43)/SUMIFS($F$6:$F$10,$E$6:$E$10,D43,$C$6:$C$10,C43)))</f>
-        <v>1</v>
-      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
+      <c r="K43" s="6"/>
       <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
-      <c r="X43" s="5"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="54"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A44" s="51"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
+      <c r="I44" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="54"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A45" s="51"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="20">
-        <f>IF(D45="overall",0,MIN(1,SUMIFS($F$19:$F$23,$E$19:$E$23,D45,$D$19:$D$23,C45)/SUMIFS($F$6:$F$10,$E$6:$E$10,D45,$C$6:$C$10,C45)))</f>
-        <v>0</v>
-      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
+      <c r="I45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="23">
+        <f>SUMIF($E$19:$E$23,I45,$K$19:$K$23)/SUMIF($E$19:$E$23,I45,$F$19:$F$23)</f>
+        <v>8</v>
+      </c>
+      <c r="K45" s="6"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
-    </row>
-    <row r="46" spans="1:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A46" s="55"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="5"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A46" s="51"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="21">
+        <f>AVERAGEIFS($E$28:$E$35,$D$28:$D$35,D46,$E$28:$E$35,"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
+      <c r="I46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="23">
+        <f>SUMIF($E$19:$E$23,I46,$K$19:$K$23)/SUMIF($E$19:$E$23,I46,$F$19:$F$23)</f>
+        <v>6.25</v>
+      </c>
+      <c r="K46" s="6"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
-    </row>
-    <row r="49" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="2"/>
-      <c r="K50" s="3"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A47" s="51"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="21">
+        <f>AVERAGEIFS($E$28:$E$35,$D$28:$D$35,D47,$E$28:$E$35,"&gt;0")</f>
+        <v>0.75</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="23">
+        <f>SUMIF($E$19:$E$23,I47,$K$19:$K$23)/SUMIF($E$19:$E$23,I47,$F$19:$F$23)</f>
+        <v>6.4</v>
+      </c>
+      <c r="K47" s="6"/>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="52"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="21">
+        <f>AVERAGEIFS($E$28:$E$35,$D$28:$D$35,D48,$E$28:$E$35,"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
       <c r="L50" s="5"/>
-      <c r="N50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="51"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="21">
-        <f>AVERAGEIF($D$39:$D$46,D51,$E$39:$E$46)</f>
-        <v>1</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J51" s="23">
-        <f>SUMIF($E$19:$E$23,I51,$I$19:$I$23)/SUMIF($E$19:$E$23,I51,$F$19:$F$23)</f>
-        <v>50</v>
-      </c>
-      <c r="K51" s="6"/>
-      <c r="L51" s="5"/>
-      <c r="N51" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="51"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="21">
-        <f>AVERAGEIF($D$39:$D$46,D52,$E$39:$E$46)</f>
-        <v>0.75</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J52" s="23">
-        <f>SUMIF($E$19:$E$23,I52,$I$19:$I$23)/SUMIF($E$19:$E$23,I52,$F$19:$F$23)</f>
-        <v>100</v>
-      </c>
-      <c r="K52" s="6"/>
-      <c r="L52" s="5"/>
-      <c r="N52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="51"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E53" s="21">
-        <f>AVERAGEIF($D$39:$D$46,D53,$E$39:$E$46)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F53" s="5"/>
+        <f>AVERAGE(E40:E42)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
-      <c r="I53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="23">
-        <f>SUMIF($E$19:$E$23,I53,$I$19:$I$23)/SUMIF($E$19:$E$23,I53,$F$19:$F$23)</f>
-        <v>70</v>
-      </c>
+      <c r="I53" s="26">
+        <f>COUNTA(S19:S23)/2</f>
+        <v>2</v>
+      </c>
+      <c r="J53" s="5"/>
       <c r="K53" s="6"/>
-      <c r="L53" s="5"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="51"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2851,9 +3038,8 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="6"/>
-      <c r="L54" s="5"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="51"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2862,290 +3048,102 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="6"/>
-      <c r="L55" s="5"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="51"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="15" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J56" s="23">
-        <f>SUMIF($E$19:$E$23,I56,$K$19:$K$23)/SUMIF($E$19:$E$23,I56,$F$19:$F$23)</f>
-        <v>8</v>
-      </c>
+      <c r="I56" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" s="5"/>
       <c r="K56" s="6"/>
-      <c r="L56" s="5"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="51"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="21">
-        <f>AVERAGEIFS($E$39:$E$46,$D$39:$D$46,D57,$E$39:$E$46,"&gt;0")</f>
-        <v>1</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E57" s="30">
+        <f>AVERAGE(E46:E48)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J57" s="23">
-        <f>SUMIF($E$19:$E$23,I57,$K$19:$K$23)/SUMIF($E$19:$E$23,I57,$F$19:$F$23)</f>
-        <v>6.25</v>
-      </c>
+      <c r="I57" s="25">
+        <f>SUM($I$19:$I$23)/SUM($F$19:$F$23)</f>
+        <v>88.181818181818187</v>
+      </c>
+      <c r="J57" s="5"/>
       <c r="K57" s="6"/>
-      <c r="L57" s="5"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="51"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="21">
-        <f>AVERAGEIFS($E$39:$E$46,$D$39:$D$46,D58,$E$39:$E$46,"&gt;0")</f>
-        <v>0.75</v>
-      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J58" s="23">
-        <f>SUMIF($E$19:$E$23,I58,$K$19:$K$23)/SUMIF($E$19:$E$23,I58,$F$19:$F$23)</f>
-        <v>6.4</v>
-      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
       <c r="K58" s="6"/>
-      <c r="L58" s="5"/>
-    </row>
-    <row r="59" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A59" s="52"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="21">
-        <f>AVERAGEIFS($E$39:$E$46,$D$39:$D$46,D59,$E$39:$E$46,"&gt;0")</f>
-        <v>1</v>
-      </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J63" s="2"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="51"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="21">
-        <f>AVERAGE(E51:E53)</f>
-        <v>0.75</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="26">
-        <f>COUNTA(S19:S23)/2</f>
-        <v>2</v>
-      </c>
-      <c r="J64" s="5"/>
-      <c r="K64" s="6"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="51"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="6"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="51"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="6"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="51"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J67" s="5"/>
-      <c r="K67" s="6"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="51"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="30">
-        <f>AVERAGE(E57:E59)</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="25">
-        <f>SUM($I$19:$I$23)/SUM($F$19:$F$23)</f>
-        <v>88.181818181818187</v>
-      </c>
-      <c r="J68" s="5"/>
-      <c r="K68" s="6"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="51"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="6"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="51"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="15" t="s">
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="51"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J70" s="5"/>
-      <c r="K70" s="6"/>
-    </row>
-    <row r="71" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A71" s="52"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="24">
+      <c r="J59" s="5"/>
+      <c r="K59" s="6"/>
+    </row>
+    <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="52"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="24">
         <f>SUM(K19:K23)/SUM(F19:F23)</f>
         <v>6.581818181818182</v>
       </c>
-      <c r="J71" s="8"/>
-      <c r="K71" s="9"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="K4:N4"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A63:A71"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C17:G17"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A27:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>